<commit_message>
did some initial review
</commit_message>
<xml_diff>
--- a/Testcases_AutoTools_Kavitha.xlsx
+++ b/Testcases_AutoTools_Kavitha.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siva\git\AutoTools-TCs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
@@ -10,14 +15,48 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Siva</author>
+  </authors>
+  <commentList>
+    <comment ref="B4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Siva:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+some test comment</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
@@ -205,8 +244,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +260,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -243,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,6 +327,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -275,14 +344,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,21 +663,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
@@ -616,7 +689,7 @@
     <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,10 +702,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
@@ -643,7 +716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
@@ -651,59 +724,73 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.5" customHeight="1">
-      <c r="A4">
+    <row r="4" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30">
-      <c r="E5" s="11" t="s">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" ht="30">
-      <c r="E6" s="4" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="E7" t="s">
+      <c r="G6" s="17"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="10" spans="1:9" ht="45">
+      <c r="F7" s="14"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -713,52 +800,52 @@
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="13" t="s">
+      <c r="F10" s="8"/>
+      <c r="G10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9" t="s">
+      <c r="H10" s="12"/>
+      <c r="I10" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="E11" s="11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="8" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" ht="30">
+      <c r="G11" s="9"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="G13" s="9"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="16" spans="1:9" ht="30">
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -768,68 +855,68 @@
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9" t="s">
+      <c r="H16" s="12"/>
+      <c r="I16" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30">
-      <c r="E17" s="11" t="s">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E17" s="8" t="s">
         <v>37</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" ht="30">
+      <c r="G17" s="9"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="G18" s="9"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="G19" s="9"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>27</v>
       </c>
       <c r="F20" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="G22" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -842,41 +929,41 @@
       <c r="E25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13" t="s">
+      <c r="F25" s="10"/>
+      <c r="G25" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9" t="s">
+      <c r="H25" s="12"/>
+      <c r="I25" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="F26" s="10"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="F27" s="10"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E28" s="4"/>
       <c r="F28" s="3"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1">
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -886,46 +973,46 @@
       <c r="C30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="12" t="s">
+      <c r="G30" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="9" t="s">
+      <c r="H30" s="11"/>
+      <c r="I30" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30">
-      <c r="E31" s="11" t="s">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E31" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F31" s="4"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" ht="30">
+      <c r="G31" s="10"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="12"/>
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="G32" s="10"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" s="4"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="36" spans="1:9" ht="45">
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="12"/>
+    </row>
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6</v>
       </c>
@@ -935,52 +1022,52 @@
       <c r="C36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="9" t="s">
+      <c r="H36" s="11"/>
+      <c r="I36" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30">
-      <c r="E37" s="11" t="s">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E37" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F37" s="4"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" ht="30">
+      <c r="G37" s="9"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E38" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F38" s="4"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="G38" s="9"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="4"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" ht="30">
+      <c r="G39" s="9"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E40" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G40" s="13"/>
-    </row>
-    <row r="42" spans="1:9" ht="45">
+      <c r="G40" s="9"/>
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
@@ -990,119 +1077,119 @@
       <c r="C42" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="4"/>
-      <c r="G42" s="13" t="s">
+      <c r="G42" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="9" t="s">
+      <c r="H42" s="11"/>
+      <c r="I42" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30">
-      <c r="E43" s="11" t="s">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E43" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="4"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" ht="30">
+      <c r="G43" s="9"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E44" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F44" s="4"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="G44" s="9"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" s="4"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" ht="30">
+      <c r="G45" s="9"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="12"/>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G46" s="13"/>
-    </row>
-    <row r="49" spans="1:9" ht="35.25" customHeight="1">
+      <c r="G46" s="9"/>
+    </row>
+    <row r="49" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>8</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F49" s="4"/>
-      <c r="G49" s="13" t="s">
+      <c r="G49" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="H49" s="8"/>
-      <c r="I49" s="9" t="s">
+      <c r="H49" s="11"/>
+      <c r="I49" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30">
-      <c r="E50" s="11" t="s">
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E50" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F50" s="4"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="9"/>
-    </row>
-    <row r="51" spans="1:9" ht="30">
+      <c r="G50" s="9"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="12"/>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E51" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F51" s="4"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="9"/>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="G51" s="9"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>19</v>
       </c>
       <c r="F52" s="3"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="9"/>
-    </row>
-    <row r="53" spans="1:9" ht="30">
+      <c r="G52" s="9"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="12"/>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E53" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G53" s="13"/>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>50</v>
       </c>
-      <c r="G54" s="13"/>
-    </row>
-    <row r="55" spans="1:9" ht="30">
-      <c r="E55" s="11" t="s">
+      <c r="G54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E55" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G55" s="13"/>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="G55" s="9"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9</v>
       </c>
@@ -1112,58 +1199,58 @@
       <c r="C58" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="E58" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F58" s="4"/>
-      <c r="G58" s="13" t="s">
+      <c r="G58" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H58" s="8"/>
-      <c r="I58" s="9" t="s">
+      <c r="H58" s="11"/>
+      <c r="I58" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30">
-      <c r="E59" s="11" t="s">
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E59" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F59" s="4"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="9"/>
-    </row>
-    <row r="60" spans="1:9" ht="30">
+      <c r="G59" s="9"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="12"/>
+    </row>
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E60" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F60" s="4"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="9"/>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="G60" s="9"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="12"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" s="4"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="9"/>
-    </row>
-    <row r="62" spans="1:9" ht="30">
+      <c r="G61" s="9"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="12"/>
+    </row>
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E62" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G62" s="13"/>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="G62" s="9"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>50</v>
       </c>
-      <c r="G63" s="13"/>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="G63" s="9"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>10</v>
       </c>
@@ -1174,55 +1261,57 @@
         <v>36</v>
       </c>
       <c r="D66" s="6"/>
-      <c r="E66" s="11" t="s">
+      <c r="E66" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F66" s="4"/>
-      <c r="G66" s="13" t="s">
+      <c r="G66" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="30">
-      <c r="E67" s="11" t="s">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E67" s="8" t="s">
         <v>40</v>
       </c>
       <c r="F67" s="4"/>
-      <c r="G67" s="13"/>
-    </row>
-    <row r="68" spans="1:7" ht="30">
+      <c r="G67" s="9"/>
+    </row>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="E68" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F68" s="4"/>
-      <c r="G68" s="13"/>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="G68" s="9"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" s="4"/>
-      <c r="G69" s="13"/>
-    </row>
-    <row r="70" spans="1:7" ht="30">
+      <c r="G69" s="9"/>
+    </row>
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="E70" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G70" s="13"/>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="G70" s="9"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
         <v>50</v>
       </c>
-      <c r="G71" s="13"/>
+      <c r="G71" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="G66:G71"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="G42:G46"/>
-    <mergeCell ref="G49:G55"/>
+    <mergeCell ref="H49:H52"/>
+    <mergeCell ref="I49:I52"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="I42:I45"/>
     <mergeCell ref="H58:H61"/>
     <mergeCell ref="I58:I61"/>
     <mergeCell ref="G58:G63"/>
@@ -1239,16 +1328,15 @@
     <mergeCell ref="I25:I28"/>
     <mergeCell ref="G16:G22"/>
     <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="H36:H39"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="I42:I45"/>
-    <mergeCell ref="H49:H52"/>
-    <mergeCell ref="I49:I52"/>
+    <mergeCell ref="G66:G71"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="G42:G46"/>
+    <mergeCell ref="G49:G55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made some changes to the expected Results for tc1 and tc3
</commit_message>
<xml_diff>
--- a/Testcases_AutoTools_Kavitha.xlsx
+++ b/Testcases_AutoTools_Kavitha.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siva\git\AutoTools-TCs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
@@ -15,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +24,7 @@
     <author>Siva</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -121,9 +116,6 @@
     <t>4. Click on the Sign in button.</t>
   </si>
   <si>
-    <t>Welcome page should display</t>
-  </si>
-  <si>
     <t>To verify whether an error message displays when the user enters  invalid credentials  - user name and password</t>
   </si>
   <si>
@@ -155,9 +147,6 @@
   </si>
   <si>
     <t>7. Access the Url to Auto tools website again.</t>
-  </si>
-  <si>
-    <t>Welcome page should display.</t>
   </si>
   <si>
     <t>3. Select Logout</t>
@@ -240,12 +229,18 @@
   <si>
     <t>User is taken to the User Form page.</t>
   </si>
+  <si>
+    <t>Welcome page (Landing page) should display</t>
+  </si>
+  <si>
+    <t>Welcome page (Landing page) should display.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,21 +324,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -352,9 +332,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -663,21 +658,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
@@ -689,7 +684,7 @@
     <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,10 +697,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
@@ -716,7 +711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75">
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
@@ -724,78 +719,78 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+    <row r="4" spans="1:9" ht="43.5" customHeight="1">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="11" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="18" t="s">
+    <row r="5" spans="1:9" ht="30">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="17"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="18" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="30">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="17"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="45">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
@@ -804,53 +799,53 @@
         <v>14</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
+      <c r="G10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="E11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" ht="30">
+      <c r="E12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E12" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="15"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="15"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="16" spans="1:9" ht="30">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
@@ -861,67 +856,67 @@
       <c r="F16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12" t="s">
+      <c r="G16" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="30">
       <c r="E17" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G17" s="15"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" ht="30">
       <c r="E18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="15"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="E20" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
       <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="E21" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="E22" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="15"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>10</v>
@@ -929,205 +924,205 @@
       <c r="E25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12" t="s">
+      <c r="F25" s="18"/>
+      <c r="G25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="30">
       <c r="E26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="1:9">
       <c r="E27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="1:9">
       <c r="E28" s="4"/>
       <c r="F28" s="3"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" customHeight="1">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12" t="s">
+      <c r="G30" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="13"/>
+      <c r="I30" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30">
       <c r="E31" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F31" s="4"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G31" s="18"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" spans="1:9" ht="30">
       <c r="E32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G32" s="18"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="14"/>
+    </row>
+    <row r="33" spans="1:9">
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" s="4"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="G33" s="18"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="36" spans="1:9" ht="45">
       <c r="A36">
         <v>6</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12" t="s">
+      <c r="G36" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30">
       <c r="E37" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F37" s="4"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G37" s="15"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" spans="1:9" ht="30">
       <c r="E38" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F38" s="4"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G38" s="15"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="14"/>
+    </row>
+    <row r="39" spans="1:9">
       <c r="E39" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="4"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="12"/>
-    </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G39" s="15"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="14"/>
+    </row>
+    <row r="40" spans="1:9" ht="30">
       <c r="E40" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G40" s="9"/>
-    </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="G40" s="15"/>
+    </row>
+    <row r="42" spans="1:9" ht="45">
       <c r="A42">
         <v>7</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="4"/>
-      <c r="G42" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H42" s="11"/>
-      <c r="I42" s="12" t="s">
+      <c r="G42" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H42" s="13"/>
+      <c r="I42" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30">
       <c r="E43" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F43" s="4"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="12"/>
-    </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G43" s="15"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="14"/>
+    </row>
+    <row r="44" spans="1:9" ht="30">
       <c r="E44" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F44" s="4"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="12"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G44" s="15"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="14"/>
+    </row>
+    <row r="45" spans="1:9">
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" s="4"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="12"/>
-    </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G45" s="15"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="14"/>
+    </row>
+    <row r="46" spans="1:9" ht="30">
       <c r="E46" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G46" s="9"/>
-    </row>
-    <row r="49" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="G46" s="15"/>
+    </row>
+    <row r="49" spans="1:9" ht="35.25" customHeight="1">
       <c r="A49">
         <v>8</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>10</v>
@@ -1136,65 +1131,65 @@
         <v>14</v>
       </c>
       <c r="F49" s="4"/>
-      <c r="G49" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H49" s="11"/>
-      <c r="I49" s="12" t="s">
+      <c r="G49" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H49" s="13"/>
+      <c r="I49" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="30">
       <c r="E50" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F50" s="4"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="12"/>
-    </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G50" s="15"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="14"/>
+    </row>
+    <row r="51" spans="1:9" ht="30">
       <c r="E51" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F51" s="4"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="12"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G51" s="15"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="14"/>
+    </row>
+    <row r="52" spans="1:9">
       <c r="E52" t="s">
         <v>19</v>
       </c>
       <c r="F52" s="3"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="12"/>
-    </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G52" s="15"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="14"/>
+    </row>
+    <row r="53" spans="1:9" ht="30">
       <c r="E53" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G53" s="15"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="E54" t="s">
+        <v>48</v>
+      </c>
+      <c r="G54" s="15"/>
+    </row>
+    <row r="55" spans="1:9" ht="30">
+      <c r="E55" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G53" s="9"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
-        <v>50</v>
-      </c>
-      <c r="G54" s="9"/>
-    </row>
-    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="E55" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G55" s="9"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="15"/>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58">
         <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>10</v>
@@ -1203,115 +1198,113 @@
         <v>14</v>
       </c>
       <c r="F58" s="4"/>
-      <c r="G58" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H58" s="11"/>
-      <c r="I58" s="12" t="s">
+      <c r="G58" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H58" s="13"/>
+      <c r="I58" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="30">
       <c r="E59" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F59" s="4"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="12"/>
-    </row>
-    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G59" s="15"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="14"/>
+    </row>
+    <row r="60" spans="1:9" ht="30">
       <c r="E60" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F60" s="4"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="12"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="15"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="14"/>
+    </row>
+    <row r="61" spans="1:9">
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" s="4"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="12"/>
-    </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="G61" s="15"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="14"/>
+    </row>
+    <row r="62" spans="1:9" ht="30">
       <c r="E62" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G62" s="9"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G62" s="15"/>
+    </row>
+    <row r="63" spans="1:9">
       <c r="E63" t="s">
-        <v>50</v>
-      </c>
-      <c r="G63" s="9"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="G63" s="15"/>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F66" s="4"/>
-      <c r="G66" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G66" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30">
       <c r="E67" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F67" s="4"/>
-      <c r="G67" s="9"/>
-    </row>
-    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G67" s="15"/>
+    </row>
+    <row r="68" spans="1:7" ht="30">
       <c r="E68" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F68" s="4"/>
-      <c r="G68" s="9"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G68" s="15"/>
+    </row>
+    <row r="69" spans="1:7">
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" s="4"/>
-      <c r="G69" s="9"/>
-    </row>
-    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G69" s="15"/>
+    </row>
+    <row r="70" spans="1:7" ht="30">
       <c r="E70" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G70" s="9"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G70" s="15"/>
+    </row>
+    <row r="71" spans="1:7">
       <c r="E71" t="s">
-        <v>50</v>
-      </c>
-      <c r="G71" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="G71" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H49:H52"/>
-    <mergeCell ref="I49:I52"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="H36:H39"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="I42:I45"/>
+    <mergeCell ref="G66:G71"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="G42:G46"/>
+    <mergeCell ref="G49:G55"/>
     <mergeCell ref="H58:H61"/>
     <mergeCell ref="I58:I61"/>
     <mergeCell ref="G58:G63"/>
@@ -1328,12 +1321,14 @@
     <mergeCell ref="I25:I28"/>
     <mergeCell ref="G16:G22"/>
     <mergeCell ref="G30:G33"/>
-    <mergeCell ref="G66:G71"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="G42:G46"/>
-    <mergeCell ref="G49:G55"/>
+    <mergeCell ref="H49:H52"/>
+    <mergeCell ref="I49:I52"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="I42:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>